<commit_message>
fix data type excel
</commit_message>
<xml_diff>
--- a/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ExcelTemplate/GiaoDichThanhToan_Export_Template.xlsx
+++ b/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ExcelTemplate/GiaoDichThanhToan_Export_Template.xlsx
@@ -215,9 +215,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -240,13 +237,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -535,7 +535,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,14 +543,14 @@
     <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="15" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
     <col min="7" max="8" width="19.28515625" style="2" customWidth="1"/>
     <col min="9" max="9" width="18.5703125" style="2" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" style="2" customWidth="1"/>
     <col min="11" max="11" width="24.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" style="5" customWidth="1"/>
     <col min="13" max="13" width="24" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -576,7 +576,7 @@
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -598,442 +598,442 @@
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="9"/>
-      <c r="AH3" s="9"/>
-      <c r="AI3" s="9"/>
-      <c r="AJ3" s="9"/>
-      <c r="AK3" s="9"/>
-      <c r="AL3" s="9"/>
-      <c r="AM3" s="9"/>
-      <c r="AN3" s="9"/>
-      <c r="AO3" s="9"/>
-      <c r="AP3" s="9"/>
-      <c r="AQ3" s="9"/>
-      <c r="AR3" s="9"/>
-      <c r="AS3" s="9"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="8"/>
+      <c r="AM3" s="8"/>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8"/>
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="8"/>
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="8"/>
     </row>
     <row r="4" spans="1:45" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="7"/>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="7"/>
-      <c r="AG4" s="7"/>
-      <c r="AH4" s="7"/>
-      <c r="AI4" s="7"/>
-      <c r="AJ4" s="7"/>
-      <c r="AK4" s="7"/>
-      <c r="AL4" s="7"/>
-      <c r="AM4" s="7"/>
-      <c r="AN4" s="7"/>
-      <c r="AO4" s="7"/>
-      <c r="AP4" s="7"/>
-      <c r="AQ4" s="7"/>
-      <c r="AR4" s="7"/>
-      <c r="AS4" s="7"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="6"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="6"/>
+      <c r="AQ4" s="6"/>
+      <c r="AR4" s="6"/>
+      <c r="AS4" s="6"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M5" s="8"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="9"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="9"/>
-      <c r="AK5" s="9"/>
-      <c r="AL5" s="9"/>
-      <c r="AM5" s="9"/>
-      <c r="AN5" s="9"/>
-      <c r="AO5" s="9"/>
-      <c r="AP5" s="9"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
-      <c r="AS5" s="9"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
+      <c r="AK5" s="8"/>
+      <c r="AL5" s="8"/>
+      <c r="AM5" s="8"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8"/>
+      <c r="AP5" s="8"/>
+      <c r="AQ5" s="8"/>
+      <c r="AR5" s="8"/>
+      <c r="AS5" s="8"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="9"/>
-      <c r="AF6" s="9"/>
-      <c r="AG6" s="9"/>
-      <c r="AH6" s="9"/>
-      <c r="AI6" s="9"/>
-      <c r="AJ6" s="9"/>
-      <c r="AK6" s="9"/>
-      <c r="AL6" s="9"/>
-      <c r="AM6" s="9"/>
-      <c r="AN6" s="9"/>
-      <c r="AO6" s="9"/>
-      <c r="AP6" s="9"/>
-      <c r="AQ6" s="9"/>
-      <c r="AR6" s="9"/>
-      <c r="AS6" s="9"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+      <c r="AL6" s="8"/>
+      <c r="AM6" s="8"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="8"/>
+      <c r="AP6" s="8"/>
+      <c r="AQ6" s="8"/>
+      <c r="AR6" s="8"/>
+      <c r="AS6" s="8"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M7" s="8"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
-      <c r="AF7" s="9"/>
-      <c r="AG7" s="9"/>
-      <c r="AH7" s="9"/>
-      <c r="AI7" s="9"/>
-      <c r="AJ7" s="9"/>
-      <c r="AK7" s="9"/>
-      <c r="AL7" s="9"/>
-      <c r="AM7" s="9"/>
-      <c r="AN7" s="9"/>
-      <c r="AO7" s="9"/>
-      <c r="AP7" s="9"/>
-      <c r="AQ7" s="9"/>
-      <c r="AR7" s="9"/>
-      <c r="AS7" s="9"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="8"/>
+      <c r="AJ7" s="8"/>
+      <c r="AK7" s="8"/>
+      <c r="AL7" s="8"/>
+      <c r="AM7" s="8"/>
+      <c r="AN7" s="8"/>
+      <c r="AO7" s="8"/>
+      <c r="AP7" s="8"/>
+      <c r="AQ7" s="8"/>
+      <c r="AR7" s="8"/>
+      <c r="AS7" s="8"/>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M8" s="8"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
-      <c r="AF8" s="9"/>
-      <c r="AG8" s="9"/>
-      <c r="AH8" s="9"/>
-      <c r="AI8" s="9"/>
-      <c r="AJ8" s="9"/>
-      <c r="AK8" s="9"/>
-      <c r="AL8" s="9"/>
-      <c r="AM8" s="9"/>
-      <c r="AN8" s="9"/>
-      <c r="AO8" s="9"/>
-      <c r="AP8" s="9"/>
-      <c r="AQ8" s="9"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
+      <c r="AK8" s="8"/>
+      <c r="AL8" s="8"/>
+      <c r="AM8" s="8"/>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
+      <c r="AQ8" s="8"/>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="9"/>
-      <c r="Z9" s="9"/>
-      <c r="AA9" s="9"/>
-      <c r="AB9" s="9"/>
-      <c r="AC9" s="9"/>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="9"/>
-      <c r="AF9" s="9"/>
-      <c r="AG9" s="9"/>
-      <c r="AH9" s="9"/>
-      <c r="AI9" s="9"/>
-      <c r="AJ9" s="9"/>
-      <c r="AK9" s="9"/>
-      <c r="AL9" s="9"/>
-      <c r="AM9" s="9"/>
-      <c r="AN9" s="9"/>
-      <c r="AO9" s="9"/>
-      <c r="AP9" s="9"/>
-      <c r="AQ9" s="9"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="8"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
+      <c r="AM9" s="8"/>
+      <c r="AN9" s="8"/>
+      <c r="AO9" s="8"/>
+      <c r="AP9" s="8"/>
+      <c r="AQ9" s="8"/>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M10" s="8"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="9"/>
-      <c r="AF10" s="9"/>
-      <c r="AG10" s="9"/>
-      <c r="AH10" s="9"/>
-      <c r="AI10" s="9"/>
-      <c r="AJ10" s="9"/>
-      <c r="AK10" s="9"/>
-      <c r="AL10" s="9"/>
-      <c r="AM10" s="9"/>
-      <c r="AN10" s="9"/>
-      <c r="AO10" s="9"/>
-      <c r="AP10" s="9"/>
-      <c r="AQ10" s="9"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
+      <c r="AJ10" s="8"/>
+      <c r="AK10" s="8"/>
+      <c r="AL10" s="8"/>
+      <c r="AM10" s="8"/>
+      <c r="AN10" s="8"/>
+      <c r="AO10" s="8"/>
+      <c r="AP10" s="8"/>
+      <c r="AQ10" s="8"/>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M11" s="8"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="9"/>
-      <c r="AF11" s="9"/>
-      <c r="AG11" s="9"/>
-      <c r="AH11" s="9"/>
-      <c r="AI11" s="9"/>
-      <c r="AJ11" s="9"/>
-      <c r="AK11" s="9"/>
-      <c r="AL11" s="9"/>
-      <c r="AM11" s="9"/>
-      <c r="AN11" s="9"/>
-      <c r="AO11" s="9"/>
-      <c r="AP11" s="9"/>
-      <c r="AQ11" s="9"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
+      <c r="AI11" s="8"/>
+      <c r="AJ11" s="8"/>
+      <c r="AK11" s="8"/>
+      <c r="AL11" s="8"/>
+      <c r="AM11" s="8"/>
+      <c r="AN11" s="8"/>
+      <c r="AO11" s="8"/>
+      <c r="AP11" s="8"/>
+      <c r="AQ11" s="8"/>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M12" s="8"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="9"/>
-      <c r="AI12" s="9"/>
-      <c r="AJ12" s="9"/>
-      <c r="AK12" s="9"/>
-      <c r="AL12" s="9"/>
-      <c r="AM12" s="9"/>
-      <c r="AN12" s="9"/>
-      <c r="AO12" s="9"/>
-      <c r="AP12" s="9"/>
-      <c r="AQ12" s="9"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="8"/>
+      <c r="AE12" s="8"/>
+      <c r="AF12" s="8"/>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="8"/>
+      <c r="AI12" s="8"/>
+      <c r="AJ12" s="8"/>
+      <c r="AK12" s="8"/>
+      <c r="AL12" s="8"/>
+      <c r="AM12" s="8"/>
+      <c r="AN12" s="8"/>
+      <c r="AO12" s="8"/>
+      <c r="AP12" s="8"/>
+      <c r="AQ12" s="8"/>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M13" s="8"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9"/>
-      <c r="AA13" s="9"/>
-      <c r="AB13" s="9"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="9"/>
-      <c r="AF13" s="9"/>
-      <c r="AG13" s="9"/>
-      <c r="AH13" s="9"/>
-      <c r="AI13" s="9"/>
-      <c r="AJ13" s="9"/>
-      <c r="AK13" s="9"/>
-      <c r="AL13" s="9"/>
-      <c r="AM13" s="9"/>
-      <c r="AN13" s="9"/>
-      <c r="AO13" s="9"/>
-      <c r="AP13" s="9"/>
-      <c r="AQ13" s="9"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+      <c r="AC13" s="8"/>
+      <c r="AD13" s="8"/>
+      <c r="AE13" s="8"/>
+      <c r="AF13" s="8"/>
+      <c r="AG13" s="8"/>
+      <c r="AH13" s="8"/>
+      <c r="AI13" s="8"/>
+      <c r="AJ13" s="8"/>
+      <c r="AK13" s="8"/>
+      <c r="AL13" s="8"/>
+      <c r="AM13" s="8"/>
+      <c r="AN13" s="8"/>
+      <c r="AO13" s="8"/>
+      <c r="AP13" s="8"/>
+      <c r="AQ13" s="8"/>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="9"/>
-      <c r="AI14" s="9"/>
-      <c r="AJ14" s="9"/>
-      <c r="AK14" s="9"/>
-      <c r="AL14" s="9"/>
-      <c r="AM14" s="9"/>
-      <c r="AN14" s="9"/>
-      <c r="AO14" s="9"/>
-      <c r="AP14" s="9"/>
-      <c r="AQ14" s="9"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="8"/>
+      <c r="AI14" s="8"/>
+      <c r="AJ14" s="8"/>
+      <c r="AK14" s="8"/>
+      <c r="AL14" s="8"/>
+      <c r="AM14" s="8"/>
+      <c r="AN14" s="8"/>
+      <c r="AO14" s="8"/>
+      <c r="AP14" s="8"/>
+      <c r="AQ14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
temp excel: add footer sum
</commit_message>
<xml_diff>
--- a/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ExcelTemplate/GiaoDichThanhToan_Export_Template.xlsx
+++ b/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ExcelTemplate/GiaoDichThanhToan_Export_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code-manhld-github\beautify_app_flutter\beautify_api\8.0.0\aspnet-core\src\BanHangBeautify.Web.Host\wwwroot\ExcelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSOFT\Open beauty\lucky_beauty\beautify_api\8.0.0\aspnet-core\src\BanHangBeautify.Web.Host\wwwroot\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="DanhSach" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,18 +32,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>STT</t>
-  </si>
-  <si>
-    <t>Danh sách hóa đơn</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Mã HĐ</t>
-  </si>
-  <si>
-    <t>Ngày bán</t>
   </si>
   <si>
     <t>Tên khách hàng</t>
@@ -52,26 +43,32 @@
     <t>Tổng tiền hàng</t>
   </si>
   <si>
-    <t>Tổng giảm giá</t>
+    <t>Trạng thái</t>
   </si>
   <si>
-    <t>Tổng khách phải trả</t>
+    <t>DANH SÁCH HÓA ĐƠN</t>
   </si>
   <si>
-    <t>Tổng đã thanh toán</t>
+    <t>Ngày lập hóa đơn</t>
   </si>
   <si>
-    <t>Khách nợ</t>
+    <t>Tổng phải trả</t>
   </si>
   <si>
-    <t>Trạng thái</t>
+    <t>Khách đã trả</t>
+  </si>
+  <si>
+    <t>Còn nợ</t>
+  </si>
+  <si>
+    <t>Tổng cộng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,8 +104,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +135,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,7 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -213,11 +225,43 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -503,149 +547,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS14"/>
+  <dimension ref="A1:AQ13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="19.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" style="5" customWidth="1"/>
-    <col min="13" max="13" width="24" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="33" style="12" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="25" customWidth="1"/>
+    <col min="5" max="6" width="19.28515625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="25" customWidth="1"/>
+    <col min="8" max="8" width="17" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="24" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:45" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+    <row r="1" spans="1:43" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="K2" s="7"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+    </row>
+    <row r="3" spans="1:43" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M3" s="7"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="8"/>
-      <c r="AG3" s="8"/>
-      <c r="AH3" s="8"/>
-      <c r="AI3" s="8"/>
-      <c r="AJ3" s="8"/>
-      <c r="AK3" s="8"/>
-      <c r="AL3" s="8"/>
-      <c r="AM3" s="8"/>
-      <c r="AN3" s="8"/>
-      <c r="AO3" s="8"/>
-      <c r="AP3" s="8"/>
-      <c r="AQ3" s="8"/>
-      <c r="AR3" s="8"/>
-      <c r="AS3" s="8"/>
-    </row>
-    <row r="4" spans="1:45" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="D3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="E3" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="6"/>
-      <c r="AG4" s="6"/>
-      <c r="AH4" s="6"/>
-      <c r="AI4" s="6"/>
-      <c r="AJ4" s="6"/>
-      <c r="AK4" s="6"/>
-      <c r="AL4" s="6"/>
-      <c r="AM4" s="6"/>
-      <c r="AN4" s="6"/>
-      <c r="AO4" s="6"/>
-      <c r="AP4" s="6"/>
-      <c r="AQ4" s="6"/>
-      <c r="AR4" s="6"/>
-      <c r="AS4" s="6"/>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M5" s="7"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
+      <c r="AL3" s="6"/>
+      <c r="AM3" s="6"/>
+      <c r="AN3" s="6"/>
+      <c r="AO3" s="6"/>
+      <c r="AP3" s="6"/>
+      <c r="AQ3" s="6"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="K4" s="7"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
+      <c r="AP4" s="8"/>
+      <c r="AQ4" s="8"/>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="K5" s="7"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
@@ -676,11 +747,11 @@
       <c r="AO5" s="8"/>
       <c r="AP5" s="8"/>
       <c r="AQ5" s="8"/>
-      <c r="AR5" s="8"/>
-      <c r="AS5" s="8"/>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M6" s="7"/>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="K6" s="7"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
@@ -711,11 +782,11 @@
       <c r="AO6" s="8"/>
       <c r="AP6" s="8"/>
       <c r="AQ6" s="8"/>
-      <c r="AR6" s="8"/>
-      <c r="AS6" s="8"/>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M7" s="7"/>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="K7" s="7"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
@@ -744,13 +815,11 @@
       <c r="AM7" s="8"/>
       <c r="AN7" s="8"/>
       <c r="AO7" s="8"/>
-      <c r="AP7" s="8"/>
-      <c r="AQ7" s="8"/>
-      <c r="AR7" s="8"/>
-      <c r="AS7" s="8"/>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M8" s="7"/>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="K8" s="7"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
@@ -779,11 +848,11 @@
       <c r="AM8" s="8"/>
       <c r="AN8" s="8"/>
       <c r="AO8" s="8"/>
-      <c r="AP8" s="8"/>
-      <c r="AQ8" s="8"/>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M9" s="7"/>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="K9" s="7"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
@@ -812,44 +881,68 @@
       <c r="AM9" s="8"/>
       <c r="AN9" s="8"/>
       <c r="AO9" s="8"/>
-      <c r="AP9" s="8"/>
-      <c r="AQ9" s="8"/>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M10" s="7"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="8"/>
-      <c r="AB10" s="8"/>
-      <c r="AC10" s="8"/>
-      <c r="AD10" s="8"/>
-      <c r="AE10" s="8"/>
-      <c r="AF10" s="8"/>
-      <c r="AG10" s="8"/>
-      <c r="AH10" s="8"/>
-      <c r="AI10" s="8"/>
-      <c r="AJ10" s="8"/>
-      <c r="AK10" s="8"/>
-      <c r="AL10" s="8"/>
-      <c r="AM10" s="8"/>
-      <c r="AN10" s="8"/>
-      <c r="AO10" s="8"/>
-      <c r="AP10" s="8"/>
-      <c r="AQ10" s="8"/>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M11" s="7"/>
+    </row>
+    <row r="10" spans="1:43" s="24" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="27">
+        <f>SUM(D$4:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="27">
+        <f>SUM(E$4:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="27">
+        <f>SUM(F$4:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="27">
+        <f>SUM(G$4:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="19"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
+      <c r="X10" s="23"/>
+      <c r="Y10" s="23"/>
+      <c r="Z10" s="23"/>
+      <c r="AA10" s="23"/>
+      <c r="AB10" s="23"/>
+      <c r="AC10" s="23"/>
+      <c r="AD10" s="23"/>
+      <c r="AE10" s="23"/>
+      <c r="AF10" s="23"/>
+      <c r="AG10" s="23"/>
+      <c r="AH10" s="23"/>
+      <c r="AI10" s="23"/>
+      <c r="AJ10" s="23"/>
+      <c r="AK10" s="23"/>
+      <c r="AL10" s="23"/>
+      <c r="AM10" s="23"/>
+      <c r="AN10" s="23"/>
+      <c r="AO10" s="23"/>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="K11" s="7"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
@@ -878,11 +971,11 @@
       <c r="AM11" s="8"/>
       <c r="AN11" s="8"/>
       <c r="AO11" s="8"/>
-      <c r="AP11" s="8"/>
-      <c r="AQ11" s="8"/>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M12" s="7"/>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="K12" s="7"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
@@ -911,11 +1004,11 @@
       <c r="AM12" s="8"/>
       <c r="AN12" s="8"/>
       <c r="AO12" s="8"/>
-      <c r="AP12" s="8"/>
-      <c r="AQ12" s="8"/>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M13" s="7"/>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="K13" s="7"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
@@ -944,45 +1037,10 @@
       <c r="AM13" s="8"/>
       <c r="AN13" s="8"/>
       <c r="AO13" s="8"/>
-      <c r="AP13" s="8"/>
-      <c r="AQ13" s="8"/>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="M14" s="7"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
-      <c r="AC14" s="8"/>
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="8"/>
-      <c r="AF14" s="8"/>
-      <c r="AG14" s="8"/>
-      <c r="AH14" s="8"/>
-      <c r="AI14" s="8"/>
-      <c r="AJ14" s="8"/>
-      <c r="AK14" s="8"/>
-      <c r="AL14" s="8"/>
-      <c r="AM14" s="8"/>
-      <c r="AN14" s="8"/>
-      <c r="AO14" s="8"/>
-      <c r="AP14" s="8"/>
-      <c r="AQ14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>